<commit_message>
Alterado código que calcula a mutação: agora a mutação altera aleatoriamente o sinal, antes era só positivo. O valor do multiplicador, e o limite dos pesos iniciais foram colocados como parâmetros nas funções de treinamento. Nesse teste, foi atingido 100% de acertividade na porta XOR após cerca de 70 gerações. Todo: corrigir função de salvar a rede neural quando se utiliza mais de 2 neurônios na camada oculta; criar função para salvar população, para poder parar o treinamento e continuar depois; Utilizar o alorítmo genético para treinar função para leitura de dígitos escritos a mão.
</commit_message>
<xml_diff>
--- a/Porta XOR.xlsx
+++ b/Porta XOR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\Digit recog 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D9EC00-C455-4841-8765-F16B06BEFD34}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631D660D-8F64-438A-B970-92936206DB35}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{07EF8DED-47A8-4193-9B75-81AF64040C19}"/>
+    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12720" xr2:uid="{07EF8DED-47A8-4193-9B75-81AF64040C19}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>dx</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>XOR genetic</t>
+  </si>
+  <si>
+    <t>y3</t>
+  </si>
+  <si>
+    <t>y4</t>
   </si>
 </sst>
 </file>
@@ -148,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -160,6 +166,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -204,7 +213,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$J$10</c:f>
+              <c:f>Planilha1!$K$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -221,7 +230,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="triangle"/>
             <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
@@ -237,7 +246,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Planilha1!$J$12:$J$13</c:f>
+              <c:f>Planilha1!$K$12:$K$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -252,7 +261,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Planilha1!$K$12:$K$13</c:f>
+              <c:f>Planilha1!$L$12:$L$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -277,7 +286,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$K$10</c:f>
+              <c:f>Planilha1!$L$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -294,7 +303,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="x"/>
+            <c:symbol val="circle"/>
             <c:size val="12"/>
             <c:spPr>
               <a:noFill/>
@@ -308,7 +317,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>(Planilha1!$J$11,Planilha1!$J$14)</c:f>
+              <c:f>(Planilha1!$K$11,Planilha1!$K$14)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -323,7 +332,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(Planilha1!$K$11,Planilha1!$K$14)</c:f>
+              <c:f>(Planilha1!$L$11,Planilha1!$L$14)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -359,42 +368,20 @@
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:dPt>
             <c:idx val="16"/>
             <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent3"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
+              <c:symbol val="none"/>
             </c:marker>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -491,67 +478,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>-1.8043251765316852</c:v>
+                  <c:v>1.6743141062774864</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.7043979266702345</c:v>
+                  <c:v>1.5599705631900336</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.6044706768087833</c:v>
+                  <c:v>1.4456270201025805</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.5045434269473326</c:v>
+                  <c:v>1.3312834770151276</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.4046161770858816</c:v>
+                  <c:v>1.2169399339276747</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.3046889272244306</c:v>
+                  <c:v>1.1025963908402217</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-1.2047616773629797</c:v>
+                  <c:v>0.98825284775276867</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1.1048344275015287</c:v>
+                  <c:v>0.8739093046653158</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-1.004907177640078</c:v>
+                  <c:v>0.75956576157786282</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.9049799277786269</c:v>
+                  <c:v>0.64522221849040984</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.80505267791717594</c:v>
+                  <c:v>0.53087867540295675</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.70512542805572498</c:v>
+                  <c:v>0.41653513231550382</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.60519817819427402</c:v>
+                  <c:v>0.30219158922805084</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.50527092833282305</c:v>
+                  <c:v>0.18784804614059783</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.40534367847137215</c:v>
+                  <c:v>7.3504503053144821E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.30541642860992119</c:v>
+                  <c:v>-4.083904003430814E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.20548917874847022</c:v>
+                  <c:v>-0.15518258312176111</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.10556192888701928</c:v>
+                  <c:v>-0.26952612620921407</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-5.6346790255684311E-3</c:v>
+                  <c:v>-0.38386966929666699</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9.4292570835882522E-2</c:v>
+                  <c:v>-0.49821321238411997</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.19421982069733348</c:v>
+                  <c:v>-0.61255675547157296</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -587,19 +574,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -680,67 +655,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>-1.8043690253659155</c:v>
+                  <c:v>0.51806583686456475</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.7044428528067379</c:v>
+                  <c:v>0.41483387758619128</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.6045166802475606</c:v>
+                  <c:v>0.3116019183078178</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.504590507688383</c:v>
+                  <c:v>0.20836995902944422</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.4046643351292056</c:v>
+                  <c:v>0.10513799975107077</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.3047381625700281</c:v>
+                  <c:v>1.9060404726973319E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-1.2048119900108507</c:v>
+                  <c:v>-0.10132591880567619</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1.1048858174516729</c:v>
+                  <c:v>-0.20455787808404968</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-1.0049596448924956</c:v>
+                  <c:v>-0.30778983736242321</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.90503347233331788</c:v>
+                  <c:v>-0.41102179664079669</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.80510729977414042</c:v>
+                  <c:v>-0.51425375591917022</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.70518112721496284</c:v>
+                  <c:v>-0.61748571519754369</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.60525495465578527</c:v>
+                  <c:v>-0.72071767447591728</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.50532878209660781</c:v>
+                  <c:v>-0.82394963375429064</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.40540260953743024</c:v>
+                  <c:v>-0.92718159303266423</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.30547643697825272</c:v>
+                  <c:v>-1.0304135523110378</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.20555026441907517</c:v>
+                  <c:v>-1.1336455115894113</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.10562409185989764</c:v>
+                  <c:v>-1.2368774708677848</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-5.6979193007202188E-3</c:v>
+                  <c:v>-1.3401094301461582</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9.4228253258457309E-2</c:v>
+                  <c:v>-1.4433413894245315</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.19415442581763484</c:v>
+                  <c:v>-1.546573348702905</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -749,6 +724,360 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-A212-47D4-BF84-9568FD0C82DC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Planilha1!$E$2:$E$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.70000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.60000000000000009</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.50000000000000011</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.40000000000000013</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.30000000000000016</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.20000000000000015</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.10000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1.3877787807814457E-16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.9999999999999867E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.19999999999999987</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.29999999999999988</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.39999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.49999999999999989</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.59999999999999987</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.69999999999999984</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.79999999999999982</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.8999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.99999999999999978</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Planilha1!$H$2:$H$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.25019942378725951</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.15898694023638998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.7774456685520568E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.3438026865348956E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.11465051041621838</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.2058629939670879</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.29707547751795738</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.38828796106882685</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.47950044461969638</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.57071292817056585</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.66192541172143537</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.7531378952723049</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.84435037882317432</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.93556286237404396</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1.0267753459249134</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-1.1179878294757828</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-1.2092003130266524</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-1.3004127965775218</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-1.3916252801283913</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-1.4828377636792609</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-1.5740502472301303</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6817-4C2E-9D76-C2165CA808D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Planilha1!$E$2:$E$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.70000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.60000000000000009</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.50000000000000011</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.40000000000000013</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.30000000000000016</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.20000000000000015</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.10000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1.3877787807814457E-16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.9999999999999867E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.19999999999999987</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.29999999999999988</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.39999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.49999999999999989</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.59999999999999987</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.69999999999999984</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.79999999999999982</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.8999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.99999999999999978</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Planilha1!$I$2:$I$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.76917138190798728</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.65321354416609423</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.53725570642420106</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.42129786868230773</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.30534003094041462</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.18938219319852145</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.342435545662826E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-4.2533482285264886E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.1584913200271581</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.27444915776905132</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.39040699551094454</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.50636483325283765</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.62232267099473093</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.7382805087366241</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.85423834647851737</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.97019618422041054</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-1.0861540219623036</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-1.2021118597041969</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-1.3180696974460901</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-1.4340275351879832</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-1.5499853729298763</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-6817-4C2E-9D76-C2165CA808D6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1499,13 +1828,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>346710</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>184785</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>70485</xdr:rowOff>
@@ -1833,21 +2162,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE6CB9E0-BD84-4481-9308-26EF876DC654}">
-  <dimension ref="A1:U22"/>
+  <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="15.140625" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1863,496 +2193,670 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="3">
+      <c r="L1" s="3">
         <v>1</v>
       </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="3">
+      <c r="M1" s="4"/>
+      <c r="N1" s="3">
         <v>2</v>
       </c>
-      <c r="N1" s="4"/>
-      <c r="Q1" s="1" t="s">
+      <c r="O1" s="4"/>
+      <c r="R1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="2">
+      <c r="S1" s="5">
         <v>1</v>
       </c>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2">
+      <c r="T1" s="5"/>
+      <c r="U1" s="5">
         <v>2</v>
       </c>
-      <c r="U1" s="2"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V1" s="5"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E2">
         <v>-1</v>
       </c>
       <c r="F2">
+        <f xml:space="preserve"> (-$L$6 - $L$4 * E2) / $L$5</f>
+        <v>1.6743141062774864</v>
+      </c>
+      <c r="G2">
         <f xml:space="preserve"> (-$M$6 - $M$4 * E2) / $M$5</f>
-        <v>-1.8043251765316852</v>
-      </c>
-      <c r="G2">
+        <v>0.51806583686456475</v>
+      </c>
+      <c r="H2">
         <f xml:space="preserve"> (-$N$6 - $N$4 * E2) / $N$5</f>
-        <v>-1.8043690253659155</v>
-      </c>
-      <c r="J2" s="1" t="s">
+        <v>0.25019942378725951</v>
+      </c>
+      <c r="I2">
+        <f xml:space="preserve"> (-$O$6 - $O$4 * E2) / $O$5</f>
+        <v>0.76917138190798728</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L2" s="2">
         <v>0</v>
       </c>
-      <c r="L2" s="1">
+      <c r="M2" s="2">
         <v>1</v>
       </c>
-      <c r="M2" s="1">
+      <c r="N2" s="2">
         <v>0</v>
       </c>
-      <c r="N2" s="1">
+      <c r="O2" s="2">
         <v>1</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="1">
+      <c r="S2" s="2">
         <v>0</v>
       </c>
-      <c r="S2" s="1">
+      <c r="T2" s="2">
         <v>1</v>
       </c>
-      <c r="T2" s="1">
+      <c r="U2" s="2">
         <v>0</v>
       </c>
-      <c r="U2" s="1">
+      <c r="V2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E3">
-        <f>E2+$B$1</f>
+        <f t="shared" ref="E3:E22" si="0">E2+$B$1</f>
         <v>-0.9</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F22" si="0" xml:space="preserve"> (-$M$6 - $M$4 * E3) / $M$5</f>
-        <v>-1.7043979266702345</v>
+        <f t="shared" ref="F3:F22" si="1" xml:space="preserve"> (-$L$6 - $L$4 * E3) / $L$5</f>
+        <v>1.5599705631900336</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G22" si="1" xml:space="preserve"> (-$N$6 - $N$4 * E3) / $N$5</f>
-        <v>-1.7044428528067379</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" ref="G3:G22" si="2" xml:space="preserve"> (-$M$6 - $M$4 * E3) / $M$5</f>
+        <v>0.41483387758619128</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H22" si="3" xml:space="preserve"> (-$N$6 - $N$4 * E3) / $N$5</f>
+        <v>0.15898694023638998</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I22" si="4" xml:space="preserve"> (-$O$6 - $O$4 * E3) / $O$5</f>
+        <v>0.65321354416609423</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E4">
-        <f>E3+$B$1</f>
+        <f t="shared" si="0"/>
         <v>-0.8</v>
       </c>
       <c r="F4">
+        <f t="shared" si="1"/>
+        <v>1.4456270201025805</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>0.3116019183078178</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="3"/>
+        <v>6.7774456685520568E-2</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="4"/>
+        <v>0.53725570642420106</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>4.3077090260090776</v>
+      </c>
+      <c r="M4">
+        <v>-12.044477041556039</v>
+      </c>
+      <c r="N4">
+        <v>8.2679240230700195</v>
+      </c>
+      <c r="O4">
+        <v>-14.85089138709381</v>
+      </c>
+      <c r="R4" s="2">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>3.629248593863613</v>
+      </c>
+      <c r="T4">
+        <v>3.561272733019516</v>
+      </c>
+      <c r="U4">
+        <v>4.2003157898753063</v>
+      </c>
+      <c r="V4">
+        <v>-4.2257463611087909</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E5">
         <f t="shared" si="0"/>
-        <v>-1.6044706768087833</v>
-      </c>
-      <c r="G4">
+        <v>-0.70000000000000007</v>
+      </c>
+      <c r="F5">
         <f t="shared" si="1"/>
-        <v>-1.6045166802475606</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>3.629248593863613</v>
-      </c>
-      <c r="L4">
-        <v>3.561272733019516</v>
-      </c>
-      <c r="M4">
-        <v>4.2003157898753063</v>
-      </c>
-      <c r="N4">
-        <v>-4.2257463611087909</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>2.0006976120536781</v>
-      </c>
-      <c r="S4">
-        <v>-2.1581358792179368</v>
-      </c>
-      <c r="T4">
-        <v>-2.30442197077438</v>
-      </c>
-      <c r="U4">
-        <v>10.58196681124836</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E5">
-        <f>E4+$B$1</f>
-        <v>-0.70000000000000007</v>
-      </c>
-      <c r="F5">
+        <v>1.3312834770151276</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>0.20836995902944422</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="3"/>
+        <v>-2.3438026865348956E-2</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="4"/>
+        <v>0.42129786868230773</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>3.7673391165729639</v>
+      </c>
+      <c r="M5">
+        <v>-11.667391693183999</v>
+      </c>
+      <c r="N5">
+        <v>9.0644654121921491</v>
+      </c>
+      <c r="O5">
+        <v>-12.80714756008984</v>
+      </c>
+      <c r="R5" s="2">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>-3.6298326954250069</v>
+      </c>
+      <c r="T5">
+        <v>-3.56036984788128</v>
+      </c>
+      <c r="U5">
+        <v>-4.2033737501022399</v>
+      </c>
+      <c r="V5">
+        <v>4.2288684264437837</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E6">
         <f t="shared" si="0"/>
-        <v>-1.5045434269473326</v>
-      </c>
-      <c r="G5">
+        <v>-0.60000000000000009</v>
+      </c>
+      <c r="F6">
         <f t="shared" si="1"/>
-        <v>-1.504590507688383</v>
-      </c>
-      <c r="J5" s="1">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>-3.6298326954250069</v>
-      </c>
-      <c r="L5">
-        <v>-3.56036984788128</v>
-      </c>
-      <c r="M5">
-        <v>-4.2033737501022399</v>
-      </c>
-      <c r="N5">
-        <v>4.2288684264437837</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>1</v>
-      </c>
-      <c r="R5">
-        <v>5.251839921644315</v>
-      </c>
-      <c r="S5">
-        <v>-5.0288135310425934</v>
-      </c>
-      <c r="T5">
-        <v>-2.2119609319503</v>
-      </c>
-      <c r="U5">
-        <v>10.30994477848712</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E6">
-        <f>E5+$B$1</f>
-        <v>-0.60000000000000009</v>
-      </c>
-      <c r="F6">
+        <v>1.2169399339276747</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>0.10513799975107077</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="3"/>
+        <v>-0.11465051041621838</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="4"/>
+        <v>0.30534003094041462</v>
+      </c>
+      <c r="K6" s="2">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>-2</v>
+      </c>
+      <c r="M6">
+        <v>-6</v>
+      </c>
+      <c r="N6">
+        <v>6</v>
+      </c>
+      <c r="O6">
+        <v>-5</v>
+      </c>
+      <c r="R6" s="2">
+        <v>2</v>
+      </c>
+      <c r="S6">
+        <v>3.3488218290292271</v>
+      </c>
+      <c r="T6">
+        <v>-3.271751841359626</v>
+      </c>
+      <c r="U6">
+        <v>-3.3839372938065702</v>
+      </c>
+      <c r="V6">
+        <v>3.4046928399142722</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E7">
         <f t="shared" si="0"/>
-        <v>-1.4046161770858816</v>
-      </c>
-      <c r="G6">
+        <v>-0.50000000000000011</v>
+      </c>
+      <c r="F7">
         <f t="shared" si="1"/>
-        <v>-1.4046643351292056</v>
-      </c>
-      <c r="J6" s="1">
+        <v>1.1025963908402217</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>1.9060404726973319E-3</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="3"/>
+        <v>-0.2058629939670879</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="4"/>
+        <v>0.18938219319852145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>-0.40000000000000013</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>0.98825284775276867</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>-0.10132591880567619</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="3"/>
+        <v>-0.29707547751795738</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="4"/>
+        <v>7.342435545662826E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>-0.30000000000000016</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>0.8739093046653158</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>-0.20455787808404968</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="3"/>
+        <v>-0.38828796106882685</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="4"/>
+        <v>-4.2533482285264886E-2</v>
+      </c>
+      <c r="K9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>-0.20000000000000015</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0.75956576157786282</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>-0.30778983736242321</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="3"/>
+        <v>-0.47950044461969638</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="4"/>
+        <v>-0.1584913200271581</v>
+      </c>
+      <c r="K10" t="s">
+        <v>8</v>
+      </c>
+      <c r="L10" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" t="s">
         <v>2</v>
       </c>
-      <c r="K6">
-        <v>3.3488218290292271</v>
-      </c>
-      <c r="L6">
-        <v>-3.271751841359626</v>
-      </c>
-      <c r="M6">
-        <v>-3.3839372938065702</v>
-      </c>
-      <c r="N6">
-        <v>3.4046928399142722</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>2</v>
-      </c>
-      <c r="R6">
-        <v>2.5</v>
-      </c>
-      <c r="S6">
-        <v>2.5</v>
-      </c>
-      <c r="T6">
-        <v>3</v>
-      </c>
-      <c r="U6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E7">
-        <f>E6+$B$1</f>
-        <v>-0.50000000000000011</v>
-      </c>
-      <c r="F7">
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E11">
         <f t="shared" si="0"/>
-        <v>-1.3046889272244306</v>
-      </c>
-      <c r="G7">
+        <v>-0.10000000000000014</v>
+      </c>
+      <c r="F11">
         <f t="shared" si="1"/>
-        <v>-1.3047381625700281</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E8">
-        <f>E7+$B$1</f>
-        <v>-0.40000000000000013</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>-1.2047616773629797</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="1"/>
-        <v>-1.2048119900108507</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E9">
-        <f>E8+$B$1</f>
-        <v>-0.30000000000000016</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>-1.1048344275015287</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="1"/>
-        <v>-1.1048858174516729</v>
-      </c>
-      <c r="J9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E10">
-        <f>E9+$B$1</f>
-        <v>-0.20000000000000015</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>-1.004907177640078</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="1"/>
-        <v>-1.0049596448924956</v>
-      </c>
-      <c r="J10" t="s">
-        <v>8</v>
-      </c>
-      <c r="K10" t="s">
-        <v>9</v>
-      </c>
-      <c r="L10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E11">
-        <f>E10+$B$1</f>
-        <v>-0.10000000000000014</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>-0.9049799277786269</v>
+        <v>0.64522221849040984</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
-        <v>-0.90503347233331788</v>
-      </c>
-      <c r="J11">
-        <v>-1</v>
+        <f t="shared" si="2"/>
+        <v>-0.41102179664079669</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="3"/>
+        <v>-0.57071292817056585</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="4"/>
+        <v>-0.27444915776905132</v>
       </c>
       <c r="K11">
         <v>-1</v>
       </c>
       <c r="L11">
+        <v>-1</v>
+      </c>
+      <c r="M11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E12">
-        <f>E11+$B$1</f>
+        <f t="shared" si="0"/>
         <v>-1.3877787807814457E-16</v>
       </c>
       <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0.53087867540295675</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>-0.51425375591917022</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="3"/>
+        <v>-0.66192541172143537</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="4"/>
+        <v>-0.39040699551094454</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>-1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E13">
         <f t="shared" si="0"/>
-        <v>-0.80505267791717594</v>
-      </c>
-      <c r="G12">
+        <v>9.9999999999999867E-2</v>
+      </c>
+      <c r="F13">
         <f t="shared" si="1"/>
-        <v>-0.80510729977414042</v>
-      </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="K12">
+        <v>0.41653513231550382</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>-0.61748571519754369</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="3"/>
+        <v>-0.7531378952723049</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="4"/>
+        <v>-0.50636483325283765</v>
+      </c>
+      <c r="K13">
         <v>-1</v>
-      </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E13">
-        <f>E12+$B$1</f>
-        <v>9.9999999999999867E-2</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>-0.70512542805572498</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="1"/>
-        <v>-0.70518112721496284</v>
-      </c>
-      <c r="J13">
-        <v>-1</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
       </c>
       <c r="L13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E14">
-        <f>E13+$B$1</f>
+        <f t="shared" si="0"/>
         <v>0.19999999999999987</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
-        <v>-0.60519817819427402</v>
+        <f t="shared" si="1"/>
+        <v>0.30219158922805084</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
-        <v>-0.60525495465578527</v>
-      </c>
-      <c r="J14">
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>-0.72071767447591728</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="3"/>
+        <v>-0.84435037882317432</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="4"/>
+        <v>-0.62232267099473093</v>
       </c>
       <c r="K14">
         <v>1</v>
       </c>
       <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="E15">
-        <f>E14+$B$1</f>
+        <f t="shared" si="0"/>
         <v>0.29999999999999988</v>
       </c>
       <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0.18784804614059783</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>-0.82394963375429064</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="3"/>
+        <v>-0.93556286237404396</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="4"/>
+        <v>-0.7382805087366241</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E16">
         <f t="shared" si="0"/>
-        <v>-0.50527092833282305</v>
-      </c>
-      <c r="G15">
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="F16">
         <f t="shared" si="1"/>
-        <v>-0.50532878209660781</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E16">
-        <f>E15+$B$1</f>
-        <v>0.39999999999999991</v>
-      </c>
-      <c r="F16">
+        <v>7.3504503053144821E-2</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>-0.92718159303266423</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="3"/>
+        <v>-1.0267753459249134</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="4"/>
+        <v>-0.85423834647851737</v>
+      </c>
+    </row>
+    <row r="17" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E17">
         <f t="shared" si="0"/>
-        <v>-0.40534367847137215</v>
-      </c>
-      <c r="G16">
+        <v>0.49999999999999989</v>
+      </c>
+      <c r="F17">
         <f t="shared" si="1"/>
-        <v>-0.40540260953743024</v>
-      </c>
-    </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E17">
-        <f>E16+$B$1</f>
-        <v>0.49999999999999989</v>
-      </c>
-      <c r="F17">
+        <v>-4.083904003430814E-2</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>-1.0304135523110378</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="3"/>
+        <v>-1.1179878294757828</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="4"/>
+        <v>-0.97019618422041054</v>
+      </c>
+    </row>
+    <row r="18" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E18">
         <f t="shared" si="0"/>
-        <v>-0.30541642860992119</v>
-      </c>
-      <c r="G17">
+        <v>0.59999999999999987</v>
+      </c>
+      <c r="F18">
         <f t="shared" si="1"/>
-        <v>-0.30547643697825272</v>
-      </c>
-    </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E18">
-        <f>E17+$B$1</f>
-        <v>0.59999999999999987</v>
-      </c>
-      <c r="F18">
+        <v>-0.15518258312176111</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>-1.1336455115894113</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="3"/>
+        <v>-1.2092003130266524</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="4"/>
+        <v>-1.0861540219623036</v>
+      </c>
+    </row>
+    <row r="19" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E19">
         <f t="shared" si="0"/>
-        <v>-0.20548917874847022</v>
-      </c>
-      <c r="G18">
+        <v>0.69999999999999984</v>
+      </c>
+      <c r="F19">
         <f t="shared" si="1"/>
-        <v>-0.20555026441907517</v>
-      </c>
-    </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E19">
-        <f>E18+$B$1</f>
-        <v>0.69999999999999984</v>
-      </c>
-      <c r="F19">
+        <v>-0.26952612620921407</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>-1.2368774708677848</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="3"/>
+        <v>-1.3004127965775218</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="4"/>
+        <v>-1.2021118597041969</v>
+      </c>
+    </row>
+    <row r="20" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E20">
         <f t="shared" si="0"/>
-        <v>-0.10556192888701928</v>
-      </c>
-      <c r="G19">
+        <v>0.79999999999999982</v>
+      </c>
+      <c r="F20">
         <f t="shared" si="1"/>
-        <v>-0.10562409185989764</v>
-      </c>
-    </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E20">
-        <f>E19+$B$1</f>
-        <v>0.79999999999999982</v>
-      </c>
-      <c r="F20">
+        <v>-0.38386966929666699</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>-1.3401094301461582</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="3"/>
+        <v>-1.3916252801283913</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="4"/>
+        <v>-1.3180696974460901</v>
+      </c>
+    </row>
+    <row r="21" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E21">
         <f t="shared" si="0"/>
-        <v>-5.6346790255684311E-3</v>
-      </c>
-      <c r="G20">
+        <v>0.8999999999999998</v>
+      </c>
+      <c r="F21">
         <f t="shared" si="1"/>
-        <v>-5.6979193007202188E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E21">
-        <f>E20+$B$1</f>
-        <v>0.8999999999999998</v>
-      </c>
-      <c r="F21">
+        <v>-0.49821321238411997</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="2"/>
+        <v>-1.4433413894245315</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="3"/>
+        <v>-1.4828377636792609</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="4"/>
+        <v>-1.4340275351879832</v>
+      </c>
+    </row>
+    <row r="22" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E22">
         <f t="shared" si="0"/>
-        <v>9.4292570835882522E-2</v>
-      </c>
-      <c r="G21">
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="F22">
         <f t="shared" si="1"/>
-        <v>9.4228253258457309E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E22">
-        <f>E21+$B$1</f>
-        <v>0.99999999999999978</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="0"/>
-        <v>0.19421982069733348</v>
+        <v>-0.61255675547157296</v>
       </c>
       <c r="G22">
-        <f t="shared" si="1"/>
-        <v>0.19415442581763484</v>
+        <f t="shared" si="2"/>
+        <v>-1.546573348702905</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="3"/>
+        <v>-1.5740502472301303</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="4"/>
+        <v>-1.5499853729298763</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -2363,8 +2867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA4518B2-3C71-492B-A0A0-85F3AADA3711}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2378,19 +2882,19 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="5">
         <v>1</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5">
         <v>2</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="5"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -2474,84 +2978,84 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="5">
         <v>1</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2">
+      <c r="C10" s="5"/>
+      <c r="D10" s="5">
         <v>2</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <v>0</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <v>1</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="2">
         <v>0</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="2">
         <v>0</v>
       </c>
       <c r="B13">
-        <v>2.0006976120536781</v>
+        <v>4.3077090260090776</v>
       </c>
       <c r="C13">
-        <v>-2.1581358792179368</v>
+        <v>-12.044477041556039</v>
       </c>
       <c r="D13">
-        <v>-2.30442197077438</v>
+        <v>8.2679240230700195</v>
       </c>
       <c r="E13">
-        <v>10.58196681124836</v>
+        <v>-14.85089138709381</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="2">
         <v>1</v>
       </c>
       <c r="B14">
-        <v>5.251839921644315</v>
+        <v>3.7673391165729639</v>
       </c>
       <c r="C14">
-        <v>-5.0288135310425934</v>
+        <v>-11.667391693183999</v>
       </c>
       <c r="D14">
-        <v>-2.2119609319503</v>
+        <v>9.0644654121921491</v>
       </c>
       <c r="E14">
-        <v>10.30994477848712</v>
+        <v>-12.80714756008984</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="2">
         <v>2</v>
       </c>
       <c r="B15">
-        <v>2.5</v>
+        <v>-2</v>
       </c>
       <c r="C15">
-        <v>2.5</v>
+        <v>-6</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>